<commit_message>
refactor:  enforce strictNullChecks and strictPropertyInitialization, and noImplicitAny on ts files
</commit_message>
<xml_diff>
--- a/public/data/db-source/doc.xlsx
+++ b/public/data/db-source/doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db-source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E7909B-965D-644F-A94F-309C92A326E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B053C07D-19F7-9742-8100-D5728BD4DB6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="500" windowWidth="21200" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -576,7 +576,7 @@
         <v>20</v>
       </c>
       <c r="F5">
-        <v>1706219962</v>
+        <v>1706239962</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
refactor:  enforce strictNullChecks and strictPropertyInitialization, and noImplicitAny on ts files (#25)
* refactor:  enforce strictNullChecks and strictPropertyInitialization, and noImplicitAny on ts files

* change: internalize jszip again
</commit_message>
<xml_diff>
--- a/public/data/db-source/doc.xlsx
+++ b/public/data/db-source/doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db-source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E7909B-965D-644F-A94F-309C92A326E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B053C07D-19F7-9742-8100-D5728BD4DB6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="500" windowWidth="21200" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -576,7 +576,7 @@
         <v>20</v>
       </c>
       <c r="F5">
-        <v>1706219962</v>
+        <v>1706239962</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>